<commit_message>
adding custom multi-line chart with custom tooltip
</commit_message>
<xml_diff>
--- a/graphic_templates/highcharts_DH/highcharts_DH.xlsx
+++ b/graphic_templates/highcharts_DH/highcharts_DH.xlsx
@@ -32,25 +32,16 @@
     <t>This is default text in the copytext spreadsheet for this graphic. &lt;a href="https://docs.google.com/spreadsheets/d/{{ COPY_GOOGLE_DOC_KEY }}/edit" target="_blank"&gt;Edit this spreadsheet&lt;/a&gt; (created when you added the graphic) to update the data and text. Delete any rows you don't need, and add others as needed. Don't forget to &lt;code&gt;fab update_copy:{{ slug }}&lt;/code&gt; to update the text or visit &lt;a href="http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1" target="_top"&gt;&lt;code&gt;http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1&lt;/code&gt;&lt;/a&gt; to refresh the data every time you reload the page!</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>footnote</t>
   </si>
   <si>
     <t>source</t>
   </si>
   <si>
-    <t>something</t>
-  </si>
-  <si>
     <t>credit</t>
   </si>
   <si>
     <t>NPR</t>
-  </si>
-  <si>
-    <t>another_thing</t>
   </si>
   <si>
     <t>hdr_state</t>
@@ -65,13 +56,22 @@
     <t>Something</t>
   </si>
   <si>
-    <t>Alabama</t>
-  </si>
-  <si>
     <t>hdr_another_thing</t>
   </si>
   <si>
     <t>Another Thing</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>something</t>
+  </si>
+  <si>
+    <t>another_thing</t>
+  </si>
+  <si>
+    <t>Alabama</t>
   </si>
   <si>
     <t>2</t>
@@ -337,7 +337,7 @@
     </row>
     <row r="4" ht="33.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -367,7 +367,7 @@
     </row>
     <row r="5" ht="33.0" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -397,10 +397,10 @@
     </row>
     <row r="6" ht="33.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -457,10 +457,10 @@
     </row>
     <row r="8" ht="33.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -489,10 +489,10 @@
     </row>
     <row r="9" ht="33.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -521,10 +521,10 @@
     </row>
     <row r="10" ht="33.0" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -853,13 +853,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -887,7 +887,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>20</v>

</xml_diff>